<commit_message>
Actualizacion,orden y plan arreglados.
</commit_message>
<xml_diff>
--- a/Gestion_Proyecto/Plan_Releases.xlsx
+++ b/Gestion_Proyecto/Plan_Releases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="PLANEAMIENTO" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
-  <si>
-    <t>ID_US</t>
-  </si>
-  <si>
-    <t>USER_STORY</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>TAREAS</t>
   </si>
@@ -96,6 +90,78 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Horas</t>
+  </si>
+  <si>
+    <t>Preparar el sistema de integracion continua</t>
+  </si>
+  <si>
+    <t>Crear el Esqueleto del sistema</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Hacer conexiones con la DB</t>
+  </si>
+  <si>
+    <t>Mostrar una lista de usuarios y vehiculos alamcenados en la DB,vista simple</t>
+  </si>
+  <si>
+    <t>Crear la funcion para registrar conductores y vehiculos</t>
+  </si>
+  <si>
+    <t>Crear sistema para insertar y actualizar datos sobre los conductores y vehiculos</t>
+  </si>
+  <si>
+    <t>Implementar una la lista de opciones para el usuario y vehiculo</t>
+  </si>
+  <si>
+    <t>Implementar un sistema de autenticion de usuario</t>
+  </si>
+  <si>
+    <t>Soporte grafico en el cliente</t>
+  </si>
+  <si>
+    <t>Implementar vista de estado de los Conductores y vehiculos</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Minimal Working Version</t>
+  </si>
+  <si>
+    <t>Introducir datos de conductores y vehiculos</t>
+  </si>
+  <si>
+    <t>Hacer un diseño de las zonas de insercion y modificacionde datos con sistemas graficos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementar vista de la asignacion de vehiculos y modificacion de estados  </t>
+  </si>
+  <si>
+    <t>Asignar un Vehiculo a un Conductor</t>
+  </si>
+  <si>
+    <t>Modificar estado de un conductor y vehiculo</t>
+  </si>
+  <si>
+    <t>Plug in the real data</t>
+  </si>
+  <si>
+    <t>Release 1</t>
+  </si>
+  <si>
+    <t>Version Estable</t>
   </si>
 </sst>
 </file>
@@ -119,7 +185,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,10 +198,63 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -145,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -166,14 +285,30 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,23 +613,319 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C2"/>
+  <dimension ref="A4:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="80.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="13">
         <v>1</v>
       </c>
+      <c r="E5" s="12">
+        <v>2</v>
+      </c>
+      <c r="F5" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="13">
+        <v>30</v>
+      </c>
+      <c r="E6" s="12">
+        <v>50</v>
+      </c>
+      <c r="F6" s="12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>1</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18">
+        <v>3</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>2</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="23">
+        <v>3</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>3</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="23">
+        <v>7</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>4</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="18">
+        <v>6</v>
+      </c>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>5</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="23">
+        <v>4</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>6</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="23">
+        <v>3</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>7</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="23">
+        <v>4</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>5</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19">
+        <v>10</v>
+      </c>
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>6</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="19">
+        <v>15</v>
+      </c>
+      <c r="F16" s="19"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>7</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="19">
+        <v>10</v>
+      </c>
+      <c r="F17" s="19"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>8</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19">
+        <v>15</v>
+      </c>
+      <c r="F18" s="19"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
+        <v>9</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>10</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>11</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
     </row>
   </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -503,7 +934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -517,140 +948,140 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>3</v>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>15</v>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>4</v>
-      </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>6</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
-        <v>5</v>
-      </c>
-      <c r="B8" s="9" t="s">
+      <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="2" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="2" t="s">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>6</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>7</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>17</v>
+      <c r="B13" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>8</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>18</v>
+      <c r="B14" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>9</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>19</v>
+      <c r="B15" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>